<commit_message>
Tele2 new web page setup
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D235"/>
+  <dimension ref="A1:D284"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5791,6 +5791,1173 @@
         </is>
       </c>
     </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy S20 Ultra Dual SIM Cosmic Black</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>GALAXY S20 ULTRA</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+iPhone 11 64GB  
+</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>APPLE</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>IPHONE 11</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>64GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Iphone 11 Pro 64GB
+</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>APPLE</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>IPHONE 11 PRO</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>64GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+iPhone 7 32 GB
+</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>APPLE</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>IPHONE 7</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>32GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+iPhone 8 64 GB
+</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>APPLE</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>IPHONE 8</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>64GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+iPhone XR 64 GB
+</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>APPLE</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>IPHONE XR</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>64GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+iPhone XS 64 GB 
+</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>APPLE</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>IPHONE XS</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>64GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+iPhone XS Max 64 GB 
+</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>APPLE</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>IPHONE XS MAX</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>64GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+CAT S52 Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>S52</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+CAT S61 Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>S61</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Doro 632 Single SIM
+</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>DORO</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>632</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Huawei P Smart Pro Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>HUAWEI</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>P SMART PRO</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Huawei  P Smart Z Dual SIM 
+</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>HUAWEI</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>P SMART Z</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Huawei P30 Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>HUAWEI</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Huawei P30 Lite Dual SIM 
+</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>HUAWEI</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>P30 LITE</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Huawei P30 Pro Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>HUAWEI</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>P30 PRO</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Huawei Y6 2019 Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>HUAWEI</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Y6</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Huawei Y7 2019 Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>HUAWEI</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Y7</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy A10 Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>GALAXY A10</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy A30s Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>GALAXY A30S</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy A50 Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>GALAXY A50</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy A51 Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>GALAXY A51</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy A70 Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>GALAXY A70</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy A71
+</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>GALAXY A71</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy Fold
+</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>GALAXY FOLD</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy Note10 Dual SIM 
+</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>GALAXY NOTE 10</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy Note 10 Lite Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>GALAXY NOTE 10 LITE</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy Note10+ Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>GALAXY NOTE 10+</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy S10 Dual SIM 128GB
+</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>GALAXY S10</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy S10 Lite Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>GALAXY S10 LITE</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy S10+ Dual SIM 128 GB
+</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>GALAXY S10+</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy S20
+</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>GALAXY S20</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy S20 Ultra 5G
+</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>GALAXY S20 ULTRA</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy S20+
+</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>GALAXY S20+</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung Galaxy Z Flip
+</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>GALAXY Z FLIP</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Xiaomi Mi Note 10 Dual SIM 
+</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>XIAOMI</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>MI NOTE 10</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Xiaomi Redmi 7A Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>XIAOMI</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>REDMI 7A</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Xiaomi Redmi Note 8 Pro Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>XIAOMI</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>REDMI NOTE 8 PRO</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Xiaomi Redmi Note 8T Dual SIM
+</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>XIAOMI</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>REDMI NOTE 8T</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mobitel Apple iPhone 11 128GB White </t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>APPLE</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>IPHONE 11</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mobitel Apple iPhone 11 64GB White </t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>APPLE</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>IPHONE 11</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>64GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mobitel Apple iPhone 8 Plus 64GB Space Grey </t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>APPLE</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>IPHONE 8 PLUS</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>64GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mobitel Samsung Galaxy A70 narančasti 128GB dual SIM SM-A705F </t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>GALAXY A70</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Mobitel Samsung Galaxy S10 kraljevsko crveni 128GB dual SIM SM-G973F </t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>GALAXY S10</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung
+—Galaxy S20 DS sivi</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>GALAXY S20</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung
+—Galaxy S20 Ultra DS sivi</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>GALAXY S20 ULTRA</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Samsung
+—Galaxy S20+ DS crni</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>GALAXY S20+</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>INFONA</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mobitel XIAOMI MI 9T 6/64GB: CRNI </t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>XIAOMI</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>MI 9T</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>64GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mobitel Xiaomi Mi Note 10 6GB/128GB Zelena  </t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>XIAOMI</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>MI NOTE 10</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>